<commit_message>
ADD ALL ARTICLE AT A TIME CHANE THE CLICK  METHOD
</commit_message>
<xml_diff>
--- a/Enterprse_Suite/src/main/java/com/quickmove/TestData/TestData.xlsx
+++ b/Enterprse_Suite/src/main/java/com/quickmove/TestData/TestData.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="357">
   <si>
     <t>Article</t>
   </si>
@@ -981,9 +981,6 @@
     <t>MH-VDN-</t>
   </si>
   <si>
-    <t>TV 50"</t>
-  </si>
-  <si>
     <t>TV 60"</t>
   </si>
   <si>
@@ -1065,52 +1062,49 @@
     <t>Wine Rack</t>
   </si>
   <si>
-    <t>dfs</t>
-  </si>
-  <si>
-    <t>dfsdf</t>
-  </si>
-  <si>
-    <t>dfsdgg</t>
-  </si>
-  <si>
-    <t>sdg</t>
-  </si>
-  <si>
-    <t>gaga</t>
-  </si>
-  <si>
-    <t>agag</t>
-  </si>
-  <si>
-    <t>ggg</t>
-  </si>
-  <si>
-    <t>af</t>
-  </si>
-  <si>
-    <t>geegh</t>
-  </si>
-  <si>
-    <t>edt</t>
-  </si>
-  <si>
-    <t>dfy5</t>
-  </si>
-  <si>
-    <t>rheh</t>
-  </si>
-  <si>
-    <t>dfh</t>
-  </si>
-  <si>
-    <t>df54</t>
-  </si>
-  <si>
-    <t>hdh54</t>
-  </si>
-  <si>
-    <t>th6</t>
+    <t>FASFA</t>
+  </si>
+  <si>
+    <t>ASFG</t>
+  </si>
+  <si>
+    <t>ASGS</t>
+  </si>
+  <si>
+    <t>GASG</t>
+  </si>
+  <si>
+    <t>AGE</t>
+  </si>
+  <si>
+    <t>GSDE</t>
+  </si>
+  <si>
+    <t>TE</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>BXCBXCB</t>
+  </si>
+  <si>
+    <t>XCBXC</t>
+  </si>
+  <si>
+    <t>CB</t>
+  </si>
+  <si>
+    <t>SDFSDFS</t>
+  </si>
+  <si>
+    <t>DFSDFSD</t>
+  </si>
+  <si>
+    <t>SDFSDFSSDF</t>
+  </si>
+  <si>
+    <t>SDF</t>
   </si>
 </sst>
 </file>
@@ -1556,8 +1550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1576,7 +1570,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B2" s="10">
         <v>0.99900141442715706</v>
@@ -1584,7 +1578,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B3" s="10">
         <v>0.24975035360678927</v>
@@ -1600,7 +1594,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B5" s="10">
         <v>0.49950070721357853</v>
@@ -1608,7 +1602,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B6" s="10">
         <v>0.19980028288543139</v>
@@ -1616,7 +1610,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B7" s="10">
         <v>0.39960056577086278</v>
@@ -1632,7 +1626,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B9" s="10">
         <v>0.19980028288543139</v>
@@ -1640,7 +1634,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="B10" s="10">
         <v>0.34965049504950491</v>
@@ -1648,7 +1642,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="B11" s="10">
         <v>9.9900141442715696E-5</v>
@@ -1656,7 +1650,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="B12" s="10">
         <v>2.4975035360678923</v>
@@ -1664,7 +1658,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="B13" s="10">
         <v>0.29970042432814709</v>
@@ -1672,7 +1666,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="B14" s="10">
         <v>0.99900141442715706</v>
@@ -1680,7 +1674,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="B15" s="10">
         <v>0.14985021216407354</v>
@@ -1688,7 +1682,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="B16" s="10">
         <v>8.9910127298444123E-2</v>
@@ -1696,7 +1690,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
       <c r="B17" s="10">
         <v>0.14144261626025459</v>
@@ -1704,7 +1698,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
-        <v>315</v>
+        <v>351</v>
       </c>
       <c r="B18" s="10">
         <v>0.24975035360678927</v>
@@ -1712,7 +1706,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B19" s="10">
         <v>0.34965049504950491</v>
@@ -1720,7 +1714,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B20" s="10">
         <v>0.4495506364922206</v>
@@ -1728,7 +1722,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B21" s="10">
         <v>1.4985021216407355</v>
@@ -1736,7 +1730,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B22" s="10">
         <v>0.99900141442715706</v>
@@ -1744,7 +1738,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B23" s="10">
         <v>0.49950070721357853</v>
@@ -1752,7 +1746,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B24" s="10">
         <v>0.29970042432814709</v>
@@ -1760,7 +1754,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B25" s="10">
         <v>0.34965049504950491</v>
@@ -1768,7 +1762,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B26" s="10">
         <v>8.9910127298444123E-2</v>
@@ -1776,7 +1770,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B27" s="10">
         <v>0.14985021216407354</v>
@@ -1784,7 +1778,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B28" s="10">
         <v>9.9900141442715695E-2</v>
@@ -1792,7 +1786,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B29" s="10">
         <v>0.19980028288543139</v>
@@ -1800,7 +1794,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B30" s="10">
         <v>0.62937089108910882</v>
@@ -1808,7 +1802,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B31" s="10">
         <v>0.91908130127298449</v>
@@ -1816,7 +1810,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B32" s="10">
         <v>1.2187817256011315</v>
@@ -1824,7 +1818,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B33" s="10">
         <v>0.24975035360678927</v>
@@ -1832,7 +1826,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B34" s="10">
         <v>0.34965049504950491</v>
@@ -1840,7 +1834,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B35" s="10">
         <v>0.49950070721357853</v>
@@ -1848,7 +1842,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B36" s="10">
         <v>0.54945077793493635</v>
@@ -1856,7 +1850,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B37" s="10">
         <v>0.64935091937765199</v>
@@ -1864,7 +1858,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B38" s="10">
         <v>0.49950070721357853</v>
@@ -1872,7 +1866,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B39" s="10">
         <v>0.3196804526166902</v>
@@ -1880,7 +1874,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B40" s="10">
         <v>0.11538466336633663</v>
@@ -1888,7 +1882,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="11" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B41" s="10">
         <v>0.24975035360678927</v>
@@ -1896,7 +1890,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B42" s="10">
         <v>0.19980028288543139</v>
@@ -1904,7 +1898,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B43" s="10">
         <v>0.7092910042432814</v>
@@ -1912,7 +1906,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="11" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B44" s="10">
         <v>0.23976033946251768</v>
@@ -1920,7 +1914,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="11" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B45" s="10">
         <v>9.9900141442715696E-5</v>

</xml_diff>

<commit_message>
Added packing material script
</commit_message>
<xml_diff>
--- a/Enterprse_Suite/src/main/java/com/quickmove/TestData/TestData.xlsx
+++ b/Enterprse_Suite/src/main/java/com/quickmove/TestData/TestData.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Addarticle" sheetId="1" r:id="rId1"/>
     <sheet name="costingProfile" sheetId="17" r:id="rId2"/>
-    <sheet name="emp" sheetId="18" r:id="rId3"/>
+    <sheet name="PackingMaterial" sheetId="18" r:id="rId3"/>
     <sheet name="MasterPrefixhorizontal" sheetId="2" r:id="rId4"/>
     <sheet name="MasterPrefixvertical" sheetId="5" r:id="rId5"/>
     <sheet name="Addroom" sheetId="6" r:id="rId6"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1043" uniqueCount="904">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1059" uniqueCount="915">
   <si>
     <t>Article</t>
   </si>
@@ -2731,9 +2731,6 @@
     <t>600</t>
   </si>
   <si>
-    <t>nagendra</t>
-  </si>
-  <si>
     <t>null</t>
   </si>
   <si>
@@ -2744,6 +2741,42 @@
   </si>
   <si>
     <t>haandyman</t>
+  </si>
+  <si>
+    <t>MaterialName</t>
+  </si>
+  <si>
+    <t>QTY</t>
+  </si>
+  <si>
+    <t>Size</t>
+  </si>
+  <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>nos12</t>
+  </si>
+  <si>
+    <t>pcs</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>3e</t>
+  </si>
+  <si>
+    <t>ew</t>
+  </si>
+  <si>
+    <t>we</t>
   </si>
 </sst>
 </file>
@@ -8326,7 +8359,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -8406,10 +8439,10 @@
         <v>891</v>
       </c>
       <c r="E2" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="F2" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="G2" t="s">
         <v>896</v>
@@ -8444,16 +8477,16 @@
         <v>889</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>891</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>896</v>
@@ -8488,16 +8521,16 @@
         <v>889</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>891</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="G4" s="8" t="s">
         <v>896</v>
@@ -8532,16 +8565,16 @@
         <v>889</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>891</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="G5" s="8" t="s">
         <v>896</v>
@@ -8576,17 +8609,97 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>899</v>
+        <v>903</v>
+      </c>
+      <c r="B1" t="s">
+        <v>904</v>
+      </c>
+      <c r="C1" t="s">
+        <v>905</v>
+      </c>
+      <c r="D1" t="s">
+        <v>882</v>
+      </c>
+      <c r="E1" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>907</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>908</v>
+      </c>
+      <c r="D2" t="s">
+        <v>909</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>910</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>912</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>909</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>911</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>913</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>909</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>910</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>914</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>909</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>